<commit_message>
M03: 자료01.slxs google email 추가
</commit_message>
<xml_diff>
--- a/자료 01.xlsx
+++ b/자료 01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBE1D35-FF83-4E06-A702-8B3EC8D31485}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE44879-5E16-40ED-9CC7-9BCE91DFDEE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>이메일 주소</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,6 +43,26 @@
   </si>
   <si>
     <t>번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>google</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iskim0706@gmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iskim0706</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iskim</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -50,7 +70,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +83,14 @@
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -83,14 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -368,16 +399,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G2"/>
+  <dimension ref="B2:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="12.75" customWidth="1"/>
-    <col min="4" max="4" width="25.875" customWidth="1"/>
+    <col min="4" max="4" width="22.25" customWidth="1"/>
     <col min="5" max="5" width="14.75" customWidth="1"/>
     <col min="6" max="6" width="12.125" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
@@ -403,9 +434,32 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{E3CEE1B8-E655-484D-B4B6-F4641E80C810}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
M09: Excel file add github, gitlab
</commit_message>
<xml_diff>
--- a/자료 01.xlsx
+++ b/자료 01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE44879-5E16-40ED-9CC7-9BCE91DFDEE1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96BF8B8-2C0A-40D3-8F01-AAD298E3DD7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>이메일 주소</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +63,18 @@
   </si>
   <si>
     <t>iskim</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>github</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iskim0706</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gitlab</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -399,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G3"/>
+  <dimension ref="B2:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -454,6 +466,28 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
M10: Add hotmail address to excel file
</commit_message>
<xml_diff>
--- a/자료 01.xlsx
+++ b/자료 01.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20366"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96BF8B8-2C0A-40D3-8F01-AAD298E3DD7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C418AA-7641-4CFA-9E76-02DE25830E7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>이메일 주소</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>gitlab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>iskim0706@hotmail.com</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dsfsf</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -411,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G5"/>
+  <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -488,12 +500,27 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{E3CEE1B8-E655-484D-B4B6-F4641E80C810}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{0C6756CD-3E35-4BE8-B080-E9375111BB73}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>